<commit_message>
Modification on student enable
</commit_message>
<xml_diff>
--- a/public/student_excel/students.xlsx
+++ b/public/student_excel/students.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITz_OnYii\Desktop\schoolmates_api\school_apis\public\student_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HomePC\Desktop\schoolmates\backend\schoolmates_apis\public\student_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C478D3E1-A79C-4B0D-A9BA-6D7BDBABF59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,13 +78,13 @@
     <t>Email Address</t>
   </si>
   <si>
-    <t>Sub Class</t>
+    <t>Campus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,7 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -146,7 +147,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -427,79 +427,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="15" width="16" customWidth="1"/>
-    <col min="16" max="16" width="19.7109375" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="19.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="15" width="16" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" customWidth="1"/>
+    <col min="17" max="17" width="17.88671875" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>14</v>
@@ -511,122 +511,103 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J2" s="1"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C3" s="7"/>
-      <c r="I3" s="1"/>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J3" s="1"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C4" s="7"/>
-      <c r="I4" s="1"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J4" s="1"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C5" s="7"/>
-      <c r="I5" s="1"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J5" s="1"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C6" s="7"/>
-      <c r="I6" s="1"/>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J6" s="1"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="7"/>
-      <c r="I7" s="1"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J7" s="1"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="I8" s="1"/>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J8" s="1"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="7"/>
-      <c r="I9" s="1"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J9" s="1"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
-      <c r="I10" s="1"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J10" s="1"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="7"/>
-      <c r="I11" s="1"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J11" s="1"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="7"/>
-      <c r="I12" s="1"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J12" s="1"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C13" s="7"/>
-      <c r="I13" s="1"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J13" s="1"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C14" s="7"/>
-      <c r="I14" s="1"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J14" s="1"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="7"/>
-      <c r="I15" s="1"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J15" s="1"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="7"/>
-      <c r="I16" s="1"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J16" s="1"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-      <c r="I17" s="1"/>
+    <row r="17" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J17" s="1"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="I18" s="1"/>
+    <row r="18" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J18" s="1"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
-      <c r="I19" s="1"/>
+    <row r="19" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J19" s="1"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
-      <c r="I20" s="1"/>
+    <row r="20" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J20" s="1"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C21" s="7"/>
-      <c r="I21" s="1"/>
+    <row r="21" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J21" s="1"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="2"/>
     </row>

</xml_diff>